<commit_message>
agregando nuevamente la linea de prediccion, descripcion de las metricas, correccion de los archivos de entrada y foto de los integrantes del grupo
</commit_message>
<xml_diff>
--- a/static/files/templates/ejemplo5.xlsx
+++ b/static/files/templates/ejemplo5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skyd/epidemiologia-test/static/files/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B81C1E85-275A-E34F-B9ED-05D939DC474F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59ABD266-4D74-FE49-A981-2846A934068D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="460" windowWidth="14360" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,10 +28,10 @@
     <t>Temperatura</t>
   </si>
   <si>
-    <t>No. Busquedas</t>
+    <t>Casos</t>
   </si>
   <si>
-    <t>Año</t>
+    <t>Busquedas</t>
   </si>
 </sst>
 </file>
@@ -899,30 +899,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>2008</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <v>21.524999999999999</v>
@@ -933,7 +935,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>2008</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -947,10 +949,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>2008</v>
+        <v>3</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>21.67142857</v>
@@ -961,10 +963,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>2008</v>
+        <v>4</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C5">
         <v>22.3</v>
@@ -975,10 +977,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>2008</v>
+        <v>5</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C6">
         <v>21.15714286</v>

</xml_diff>